<commit_message>
Atualzação da minha tabela de horas trabalhadas
</commit_message>
<xml_diff>
--- a/app/Tempo-Tabalhado-Allexandre.xlsx
+++ b/app/Tempo-Tabalhado-Allexandre.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26215"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alcemirsantos/Workspace/FlutterWorkspace/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\arise-uespi\ceres\app\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540"/>
+    <workbookView xWindow="0" yWindow="456" windowWidth="28800" windowHeight="17544"/>
   </bookViews>
   <sheets>
     <sheet name="Time Sheet" sheetId="1" r:id="rId1"/>
@@ -20,20 +20,20 @@
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Time Sheet'!$7:$7</definedName>
     <definedName name="WorkweekHours">'Time Sheet'!$B$6</definedName>
   </definedNames>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
   <si>
     <t>Hours Worked</t>
   </si>
@@ -89,6 +89,12 @@
   </si>
   <si>
     <t>Dec, 28th</t>
+  </si>
+  <si>
+    <t>May 31, 2020</t>
+  </si>
+  <si>
+    <t>April 1, 2020</t>
   </si>
 </sst>
 </file>
@@ -219,7 +225,7 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
@@ -263,22 +269,25 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="7" applyFont="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="6" applyFont="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="12">
     <cellStyle name="Date" xfId="6"/>
-    <cellStyle name="Followed Hyperlink" xfId="11" builtinId="9" customBuiltin="1"/>
-    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Hiperlink" xfId="10" builtinId="8" customBuiltin="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="11" builtinId="9" customBuiltin="1"/>
     <cellStyle name="Hours" xfId="7"/>
-    <cellStyle name="Hyperlink" xfId="10" builtinId="8" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
     <cellStyle name="Phone" xfId="9"/>
     <cellStyle name="Time" xfId="8"/>
-    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Título" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Título 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Título 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Título 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Título 4" xfId="5" builtinId="19" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="4">
     <dxf>
@@ -346,8 +355,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="TimeSheet" displayName="TimeSheet" ref="B7:G29" totalsRowShown="0">
-  <autoFilter ref="B7:G29"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="TimeSheet" displayName="TimeSheet" ref="B7:G31" totalsRowShown="0">
+  <autoFilter ref="B7:G31"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Date(s)" dataCellStyle="Date"/>
     <tableColumn id="2" name="Time In" dataCellStyle="Time"/>
@@ -630,27 +639,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet1" enableFormatConditionsCalculation="0">
+  <sheetPr codeName="Sheet1">
     <tabColor theme="4"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:H29"/>
+  <dimension ref="B1:H31"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="19.95" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="2.6640625" customWidth="1"/>
     <col min="2" max="2" width="22.6640625" customWidth="1"/>
     <col min="3" max="5" width="20.6640625" customWidth="1"/>
-    <col min="6" max="6" width="15.5" customWidth="1"/>
+    <col min="6" max="6" width="15.44140625" customWidth="1"/>
     <col min="7" max="7" width="18.6640625" customWidth="1"/>
     <col min="8" max="8" width="2.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" ht="35" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:8" ht="34.950000000000003" customHeight="1" thickTop="1" x14ac:dyDescent="0.6">
       <c r="B1" s="1" t="s">
         <v>7</v>
       </c>
@@ -661,7 +670,7 @@
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
     </row>
-    <row r="2" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="8" t="s">
         <v>13</v>
       </c>
@@ -675,7 +684,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>12</v>
       </c>
@@ -683,7 +692,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="2:8" ht="35" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:8" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B4" s="10" t="s">
         <v>17</v>
       </c>
@@ -691,7 +700,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="2:8" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:8" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="2" t="s">
         <v>15</v>
       </c>
@@ -705,13 +714,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B6" s="3">
         <v>40</v>
       </c>
       <c r="C6" s="3">
         <f>SUBTOTAL(109,TimeSheet[Hours Worked])</f>
-        <v>65.500000000000014</v>
+        <v>77.500000000000014</v>
       </c>
       <c r="D6" s="3">
         <f>IFERROR(IF(C6&lt;=WorkweekHours,C6,WorkweekHours),"")</f>
@@ -719,10 +728,10 @@
       </c>
       <c r="E6" s="3">
         <f>IFERROR(C6-D6, "")</f>
-        <v>25.500000000000014</v>
-      </c>
-    </row>
-    <row r="7" spans="2:8" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+        <v>37.500000000000014</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="7" t="s">
         <v>8</v>
       </c>
@@ -742,7 +751,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="4">
         <v>43827</v>
       </c>
@@ -763,7 +772,7 @@
         <v>9.0000000000000018</v>
       </c>
     </row>
-    <row r="9" spans="2:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="4">
         <v>43828</v>
       </c>
@@ -784,7 +793,7 @@
         <v>9.0000000000000018</v>
       </c>
     </row>
-    <row r="10" spans="2:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="4">
         <v>43829</v>
       </c>
@@ -805,7 +814,7 @@
         <v>9.0000000000000018</v>
       </c>
     </row>
-    <row r="11" spans="2:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="4">
         <v>43836</v>
       </c>
@@ -826,7 +835,7 @@
         <v>9.0000000000000018</v>
       </c>
     </row>
-    <row r="12" spans="2:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="4">
         <v>43837</v>
       </c>
@@ -847,7 +856,7 @@
         <v>9.0000000000000018</v>
       </c>
     </row>
-    <row r="13" spans="2:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="4">
         <v>43838</v>
       </c>
@@ -864,7 +873,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="2:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="4">
         <v>43839</v>
       </c>
@@ -881,7 +890,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="2:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="4">
         <v>43840</v>
       </c>
@@ -898,7 +907,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="2:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="4">
         <v>43843</v>
       </c>
@@ -915,7 +924,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="4">
         <v>43844</v>
       </c>
@@ -928,7 +937,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="4">
         <v>43845</v>
       </c>
@@ -941,7 +950,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="2:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="4">
         <v>43846</v>
       </c>
@@ -958,7 +967,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="2:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="4">
         <v>43847</v>
       </c>
@@ -975,7 +984,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="4">
         <v>43850</v>
       </c>
@@ -992,7 +1001,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="2:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="4">
         <v>43851</v>
       </c>
@@ -1005,7 +1014,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="2:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B23" s="4">
         <v>43852</v>
       </c>
@@ -1018,7 +1027,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="2:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24" s="4">
         <v>43853</v>
       </c>
@@ -1035,7 +1044,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="2:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B25" s="4">
         <v>43854</v>
       </c>
@@ -1052,7 +1061,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="2:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B26" s="4">
         <v>43857</v>
       </c>
@@ -1069,7 +1078,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="2:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B27" s="4">
         <v>43858</v>
       </c>
@@ -1086,7 +1095,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="2:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B28" s="4">
         <v>43859</v>
       </c>
@@ -1107,7 +1116,7 @@
         <v>12.000000000000004</v>
       </c>
     </row>
-    <row r="29" spans="2:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B29" s="4">
         <v>43860</v>
       </c>
@@ -1126,6 +1135,44 @@
       <c r="G29" s="14">
         <f>IFERROR(IF(COUNT(TimeSheet[[#This Row],[Time In]:[Time Out]])=4,(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Lunch End]]+TimeSheet[[#This Row],[Lunch Start]]-TimeSheet[[#This Row],[Time In]],IF(AND(LEN(TimeSheet[[#This Row],[Time In]])&lt;&gt;0,LEN(TimeSheet[[#This Row],[Time Out]])&lt;&gt;0),(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Time In]],0))*24,0)</f>
         <v>8.5000000000000018</v>
+      </c>
+    </row>
+    <row r="30" spans="2:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="C30" s="13">
+        <v>0.375</v>
+      </c>
+      <c r="D30" s="13">
+        <v>0.5</v>
+      </c>
+      <c r="E30" s="13">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="F30" s="13">
+        <v>0.85416666666666663</v>
+      </c>
+      <c r="G30" s="14">
+        <f>IFERROR(IF(COUNT(TimeSheet[[#This Row],[Time In]:[Time Out]])=4,(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Lunch End]]+TimeSheet[[#This Row],[Lunch Start]]-TimeSheet[[#This Row],[Time In]],IF(AND(LEN(TimeSheet[[#This Row],[Time In]])&lt;&gt;0,LEN(TimeSheet[[#This Row],[Time Out]])&lt;&gt;0),(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Time In]],0))*24,0)</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="31" spans="2:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B31" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="C31" s="13">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="D31" s="13"/>
+      <c r="E31" s="13"/>
+      <c r="F31" s="13">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="G31" s="14">
+        <f>IFERROR(IF(COUNT(TimeSheet[[#This Row],[Time In]:[Time Out]])=4,(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Lunch End]]+TimeSheet[[#This Row],[Lunch Start]]-TimeSheet[[#This Row],[Time In]],IF(AND(LEN(TimeSheet[[#This Row],[Time In]])&lt;&gt;0,LEN(TimeSheet[[#This Row],[Time Out]])&lt;&gt;0),(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Time In]],0))*24,0)</f>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finalizado todas as requisições de Usuário
</commit_message>
<xml_diff>
--- a/app/Tempo-Tabalhado-Allexandre.xlsx
+++ b/app/Tempo-Tabalhado-Allexandre.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
   <si>
     <t>Hours Worked</t>
   </si>
@@ -95,6 +95,12 @@
   </si>
   <si>
     <t>April 1, 2020</t>
+  </si>
+  <si>
+    <t>April 4, 2020</t>
+  </si>
+  <si>
+    <t>April 5, 2020</t>
   </si>
 </sst>
 </file>
@@ -355,8 +361,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="TimeSheet" displayName="TimeSheet" ref="B7:G31" totalsRowShown="0">
-  <autoFilter ref="B7:G31"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="TimeSheet" displayName="TimeSheet" ref="B7:G33" totalsRowShown="0">
+  <autoFilter ref="B7:G33"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Date(s)" dataCellStyle="Date"/>
     <tableColumn id="2" name="Time In" dataCellStyle="Time"/>
@@ -643,10 +649,10 @@
     <tabColor theme="4"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:H31"/>
+  <dimension ref="B1:H33"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="19.95" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -720,7 +726,7 @@
       </c>
       <c r="C6" s="3">
         <f>SUBTOTAL(109,TimeSheet[Hours Worked])</f>
-        <v>77.500000000000014</v>
+        <v>88.500000000000014</v>
       </c>
       <c r="D6" s="3">
         <f>IFERROR(IF(C6&lt;=WorkweekHours,C6,WorkweekHours),"")</f>
@@ -728,7 +734,7 @@
       </c>
       <c r="E6" s="3">
         <f>IFERROR(C6-D6, "")</f>
-        <v>37.500000000000014</v>
+        <v>48.500000000000014</v>
       </c>
     </row>
     <row r="7" spans="2:8" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
@@ -1173,6 +1179,40 @@
       <c r="G31" s="14">
         <f>IFERROR(IF(COUNT(TimeSheet[[#This Row],[Time In]:[Time Out]])=4,(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Lunch End]]+TimeSheet[[#This Row],[Lunch Start]]-TimeSheet[[#This Row],[Time In]],IF(AND(LEN(TimeSheet[[#This Row],[Time In]])&lt;&gt;0,LEN(TimeSheet[[#This Row],[Time Out]])&lt;&gt;0),(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Time In]],0))*24,0)</f>
         <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="2:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B32" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="C32" s="13">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="D32" s="13"/>
+      <c r="E32" s="13"/>
+      <c r="F32" s="13">
+        <v>0.875</v>
+      </c>
+      <c r="G32" s="14">
+        <f>IFERROR(IF(COUNT(TimeSheet[[#This Row],[Time In]:[Time Out]])=4,(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Lunch End]]+TimeSheet[[#This Row],[Lunch Start]]-TimeSheet[[#This Row],[Time In]],IF(AND(LEN(TimeSheet[[#This Row],[Time In]])&lt;&gt;0,LEN(TimeSheet[[#This Row],[Time Out]])&lt;&gt;0),(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Time In]],0))*24,0)</f>
+        <v>5.0000000000000009</v>
+      </c>
+    </row>
+    <row r="33" spans="2:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B33" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="C33" s="13">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="D33" s="13"/>
+      <c r="E33" s="13"/>
+      <c r="F33" s="13">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="G33" s="14">
+        <f>IFERROR(IF(COUNT(TimeSheet[[#This Row],[Time In]:[Time Out]])=4,(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Lunch End]]+TimeSheet[[#This Row],[Lunch Start]]-TimeSheet[[#This Row],[Time In]],IF(AND(LEN(TimeSheet[[#This Row],[Time In]])&lt;&gt;0,LEN(TimeSheet[[#This Row],[Time Out]])&lt;&gt;0),(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Time In]],0))*24,0)</f>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Criado a requisição de listar as reservas do usuario
</commit_message>
<xml_diff>
--- a/app/Tempo-Tabalhado-Allexandre.xlsx
+++ b/app/Tempo-Tabalhado-Allexandre.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
   <si>
     <t>Hours Worked</t>
   </si>
@@ -101,6 +101,9 @@
   </si>
   <si>
     <t>April 5, 2020</t>
+  </si>
+  <si>
+    <t>April 6, 2020</t>
   </si>
 </sst>
 </file>
@@ -361,8 +364,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="TimeSheet" displayName="TimeSheet" ref="B7:G33" totalsRowShown="0">
-  <autoFilter ref="B7:G33"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="TimeSheet" displayName="TimeSheet" ref="B7:G34" totalsRowShown="0">
+  <autoFilter ref="B7:G34"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Date(s)" dataCellStyle="Date"/>
     <tableColumn id="2" name="Time In" dataCellStyle="Time"/>
@@ -649,10 +652,10 @@
     <tabColor theme="4"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:H33"/>
+  <dimension ref="B1:H34"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="19.95" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -726,7 +729,7 @@
       </c>
       <c r="C6" s="3">
         <f>SUBTOTAL(109,TimeSheet[Hours Worked])</f>
-        <v>88.500000000000014</v>
+        <v>92.250000000000014</v>
       </c>
       <c r="D6" s="3">
         <f>IFERROR(IF(C6&lt;=WorkweekHours,C6,WorkweekHours),"")</f>
@@ -734,7 +737,7 @@
       </c>
       <c r="E6" s="3">
         <f>IFERROR(C6-D6, "")</f>
-        <v>48.500000000000014</v>
+        <v>52.250000000000014</v>
       </c>
     </row>
     <row r="7" spans="2:8" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
@@ -1213,6 +1216,23 @@
       <c r="G33" s="14">
         <f>IFERROR(IF(COUNT(TimeSheet[[#This Row],[Time In]:[Time Out]])=4,(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Lunch End]]+TimeSheet[[#This Row],[Lunch Start]]-TimeSheet[[#This Row],[Time In]],IF(AND(LEN(TimeSheet[[#This Row],[Time In]])&lt;&gt;0,LEN(TimeSheet[[#This Row],[Time Out]])&lt;&gt;0),(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Time In]],0))*24,0)</f>
         <v>6</v>
+      </c>
+    </row>
+    <row r="34" spans="2:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B34" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="C34" s="13">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="D34" s="13"/>
+      <c r="E34" s="13"/>
+      <c r="F34" s="13">
+        <v>0.98958333333333337</v>
+      </c>
+      <c r="G34" s="14">
+        <f>IFERROR(IF(COUNT(TimeSheet[[#This Row],[Time In]:[Time Out]])=4,(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Lunch End]]+TimeSheet[[#This Row],[Lunch Start]]-TimeSheet[[#This Row],[Time In]],IF(AND(LEN(TimeSheet[[#This Row],[Time In]])&lt;&gt;0,LEN(TimeSheet[[#This Row],[Time Out]])&lt;&gt;0),(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Time In]],0))*24,0)</f>
+        <v>3.75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finalizado funcionalidades basicas do app
</commit_message>
<xml_diff>
--- a/app/Tempo-Tabalhado-Allexandre.xlsx
+++ b/app/Tempo-Tabalhado-Allexandre.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
   <si>
     <t>Hours Worked</t>
   </si>
@@ -104,6 +104,9 @@
   </si>
   <si>
     <t>April 6, 2020</t>
+  </si>
+  <si>
+    <t>April 7, 2020</t>
   </si>
 </sst>
 </file>
@@ -364,8 +367,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="TimeSheet" displayName="TimeSheet" ref="B7:G34" totalsRowShown="0">
-  <autoFilter ref="B7:G34"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="TimeSheet" displayName="TimeSheet" ref="B7:G35" totalsRowShown="0">
+  <autoFilter ref="B7:G35"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Date(s)" dataCellStyle="Date"/>
     <tableColumn id="2" name="Time In" dataCellStyle="Time"/>
@@ -652,10 +655,10 @@
     <tabColor theme="4"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:H34"/>
+  <dimension ref="B1:H35"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="G34" sqref="G34"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="19.95" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1233,6 +1236,23 @@
       <c r="G34" s="14">
         <f>IFERROR(IF(COUNT(TimeSheet[[#This Row],[Time In]:[Time Out]])=4,(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Lunch End]]+TimeSheet[[#This Row],[Lunch Start]]-TimeSheet[[#This Row],[Time In]],IF(AND(LEN(TimeSheet[[#This Row],[Time In]])&lt;&gt;0,LEN(TimeSheet[[#This Row],[Time Out]])&lt;&gt;0),(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Time In]],0))*24,0)</f>
         <v>3.75</v>
+      </c>
+    </row>
+    <row r="35" spans="2:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B35" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C35" s="13">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D35" s="13">
+        <v>2.7777777777777776E-2</v>
+      </c>
+      <c r="E35" s="13"/>
+      <c r="F35" s="13"/>
+      <c r="G35" s="14">
+        <f>IFERROR(IF(COUNT(TimeSheet[[#This Row],[Time In]:[Time Out]])=4,(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Lunch End]]+TimeSheet[[#This Row],[Lunch Start]]-TimeSheet[[#This Row],[Time In]],IF(AND(LEN(TimeSheet[[#This Row],[Time In]])&lt;&gt;0,LEN(TimeSheet[[#This Row],[Time Out]])&lt;&gt;0),(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Time In]],0))*24,0)</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Melhoria consideravel nos layouts
</commit_message>
<xml_diff>
--- a/app/Tempo-Tabalhado-Allexandre.xlsx
+++ b/app/Tempo-Tabalhado-Allexandre.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
   <si>
     <t>Hours Worked</t>
   </si>
@@ -107,6 +107,9 @@
   </si>
   <si>
     <t>April 7, 2020</t>
+  </si>
+  <si>
+    <t>April 13, 2020</t>
   </si>
 </sst>
 </file>
@@ -367,8 +370,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="TimeSheet" displayName="TimeSheet" ref="B7:G35" totalsRowShown="0">
-  <autoFilter ref="B7:G35"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="TimeSheet" displayName="TimeSheet" ref="B7:G36" totalsRowShown="0">
+  <autoFilter ref="B7:G36"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Date(s)" dataCellStyle="Date"/>
     <tableColumn id="2" name="Time In" dataCellStyle="Time"/>
@@ -655,10 +658,10 @@
     <tabColor theme="4"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:H35"/>
+  <dimension ref="B1:H36"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="L38" sqref="L38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="19.95" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -732,7 +735,7 @@
       </c>
       <c r="C6" s="3">
         <f>SUBTOTAL(109,TimeSheet[Hours Worked])</f>
-        <v>100.91666666666669</v>
+        <v>106.46666666666668</v>
       </c>
       <c r="D6" s="3">
         <f>IFERROR(IF(C6&lt;=WorkweekHours,C6,WorkweekHours),"")</f>
@@ -740,7 +743,7 @@
       </c>
       <c r="E6" s="3">
         <f>IFERROR(C6-D6, "")</f>
-        <v>60.916666666666686</v>
+        <v>66.466666666666683</v>
       </c>
     </row>
     <row r="7" spans="2:8" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
@@ -1257,6 +1260,23 @@
       <c r="G35" s="14">
         <f>IFERROR(IF(COUNT(TimeSheet[[#This Row],[Time In]:[Time Out]])=4,(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Lunch End]]+TimeSheet[[#This Row],[Lunch Start]]-TimeSheet[[#This Row],[Time In]],IF(AND(LEN(TimeSheet[[#This Row],[Time In]])&lt;&gt;0,LEN(TimeSheet[[#This Row],[Time Out]])&lt;&gt;0),(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Time In]],0))*24,0)</f>
         <v>8.6666666666666661</v>
+      </c>
+    </row>
+    <row r="36" spans="2:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B36" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="C36" s="13">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="D36" s="13"/>
+      <c r="E36" s="13"/>
+      <c r="F36" s="13">
+        <v>0.93958333333333333</v>
+      </c>
+      <c r="G36" s="14">
+        <f>IFERROR(IF(COUNT(TimeSheet[[#This Row],[Time In]:[Time Out]])=4,(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Lunch End]]+TimeSheet[[#This Row],[Lunch Start]]-TimeSheet[[#This Row],[Time In]],IF(AND(LEN(TimeSheet[[#This Row],[Time In]])&lt;&gt;0,LEN(TimeSheet[[#This Row],[Time Out]])&lt;&gt;0),(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Time In]],0))*24,0)</f>
+        <v>5.5499999999999989</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
melhoria na interface e peuqena otimização no sistema
</commit_message>
<xml_diff>
--- a/app/Tempo-Tabalhado-Allexandre.xlsx
+++ b/app/Tempo-Tabalhado-Allexandre.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
   <si>
     <t>Hours Worked</t>
   </si>
@@ -110,6 +110,12 @@
   </si>
   <si>
     <t>April 13, 2020</t>
+  </si>
+  <si>
+    <t>April 15, 2020</t>
+  </si>
+  <si>
+    <t>April 16, 2020</t>
   </si>
 </sst>
 </file>
@@ -370,8 +376,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="TimeSheet" displayName="TimeSheet" ref="B7:G36" totalsRowShown="0">
-  <autoFilter ref="B7:G36"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="TimeSheet" displayName="TimeSheet" ref="B7:G38" totalsRowShown="0">
+  <autoFilter ref="B7:G38"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Date(s)" dataCellStyle="Date"/>
     <tableColumn id="2" name="Time In" dataCellStyle="Time"/>
@@ -658,10 +664,10 @@
     <tabColor theme="4"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:H36"/>
+  <dimension ref="B1:H38"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="L38" sqref="L38"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="J38" sqref="J38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="19.95" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -735,7 +741,7 @@
       </c>
       <c r="C6" s="3">
         <f>SUBTOTAL(109,TimeSheet[Hours Worked])</f>
-        <v>106.46666666666668</v>
+        <v>110.46666666666668</v>
       </c>
       <c r="D6" s="3">
         <f>IFERROR(IF(C6&lt;=WorkweekHours,C6,WorkweekHours),"")</f>
@@ -743,7 +749,7 @@
       </c>
       <c r="E6" s="3">
         <f>IFERROR(C6-D6, "")</f>
-        <v>66.466666666666683</v>
+        <v>70.466666666666683</v>
       </c>
     </row>
     <row r="7" spans="2:8" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
@@ -1277,6 +1283,38 @@
       <c r="G36" s="14">
         <f>IFERROR(IF(COUNT(TimeSheet[[#This Row],[Time In]:[Time Out]])=4,(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Lunch End]]+TimeSheet[[#This Row],[Lunch Start]]-TimeSheet[[#This Row],[Time In]],IF(AND(LEN(TimeSheet[[#This Row],[Time In]])&lt;&gt;0,LEN(TimeSheet[[#This Row],[Time Out]])&lt;&gt;0),(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Time In]],0))*24,0)</f>
         <v>5.5499999999999989</v>
+      </c>
+    </row>
+    <row r="37" spans="2:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B37" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="C37" s="13">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="D37" s="13"/>
+      <c r="E37" s="13"/>
+      <c r="F37" s="13">
+        <v>0.875</v>
+      </c>
+      <c r="G37" s="14">
+        <f>IFERROR(IF(COUNT(TimeSheet[[#This Row],[Time In]:[Time Out]])=4,(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Lunch End]]+TimeSheet[[#This Row],[Lunch Start]]-TimeSheet[[#This Row],[Time In]],IF(AND(LEN(TimeSheet[[#This Row],[Time In]])&lt;&gt;0,LEN(TimeSheet[[#This Row],[Time Out]])&lt;&gt;0),(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Time In]],0))*24,0)</f>
+        <v>3.9999999999999991</v>
+      </c>
+    </row>
+    <row r="38" spans="2:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B38" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="C38" s="13">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="D38" s="13"/>
+      <c r="E38" s="13"/>
+      <c r="F38" s="13"/>
+      <c r="G38" s="14">
+        <f>IFERROR(IF(COUNT(TimeSheet[[#This Row],[Time In]:[Time Out]])=4,(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Lunch End]]+TimeSheet[[#This Row],[Lunch Start]]-TimeSheet[[#This Row],[Time In]],IF(AND(LEN(TimeSheet[[#This Row],[Time In]])&lt;&gt;0,LEN(TimeSheet[[#This Row],[Time Out]])&lt;&gt;0),(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Time In]],0))*24,0)</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>